<commit_message>
update rapid7 and add solarwinds
</commit_message>
<xml_diff>
--- a/chegg.xlsx
+++ b/chegg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacharles\Desktop\work\models\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C3111-B7CD-42C4-99A5-E8015B13F696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC4EF0C-A170-4023-8B1F-778177ABF9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11235" yWindow="0" windowWidth="27270" windowHeight="20985" activeTab="1" xr2:uid="{432C428B-38F2-40D4-B093-3E544D75CE3B}"/>
+    <workbookView xWindow="19755" yWindow="1560" windowWidth="18555" windowHeight="19155" activeTab="1" xr2:uid="{432C428B-38F2-40D4-B093-3E544D75CE3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,6 @@
     <t>total other income (expense)</t>
   </si>
   <si>
-    <t>ev / mc</t>
-  </si>
-  <si>
     <t>cash @ beginning of period</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>npv</t>
+  </si>
+  <si>
+    <t>ev / fcf</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -400,6 +400,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,7 +739,7 @@
   <dimension ref="B1:L47"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,11 +832,11 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8">
-        <f>L7/L4</f>
-        <v>1.9735322700508775</v>
+        <v>88</v>
+      </c>
+      <c r="L8" s="22">
+        <f>L7/Sheet2!K34</f>
+        <v>2.1166768853464135</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -890,22 +891,22 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -915,97 +916,97 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1018,10 +1019,10 @@
   <dimension ref="B1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M37" sqref="M37:M40"/>
+      <selection pane="bottomRight" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,22 +1072,22 @@
         <v>2023</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -1202,14 +1203,14 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="15"/>
@@ -1224,7 +1225,7 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="15"/>
@@ -1234,7 +1235,7 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="15"/>
@@ -1527,7 +1528,7 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F22" s="12">
         <v>-77.7</v>
@@ -1563,7 +1564,7 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -1821,7 +1822,7 @@
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29">
         <v>141.19999999999999</v>
@@ -1847,7 +1848,7 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F30">
         <f t="shared" ref="F30:H30" si="9">F29-F28</f>
@@ -1875,7 +1876,7 @@
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F31">
         <f t="shared" ref="F31:H31" si="10">F30-F29</f>
@@ -1904,7 +1905,7 @@
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F32">
         <v>75.099999999999994</v>
@@ -1933,10 +1934,10 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33" s="12">
         <f>-42.3</f>
@@ -1961,7 +1962,7 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F34">
         <f>SUM(F32:F33)</f>
@@ -1990,17 +1991,17 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M39" s="2"/>
     </row>

</xml_diff>